<commit_message>
feat: app version 2.0 - add suggestion when inputting customer - authorizer can be select by company name or company id - add new device type - add mid/tid functions - new UI
</commit_message>
<xml_diff>
--- a/sourceDocs/THONG_TIN.xlsx
+++ b/sourceDocs/THONG_TIN.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\testProject\auto-complete-docx-form\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\testProject\auto-complete-docx-form\sourceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AB9775-B243-4BCE-886F-89A6662BA67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9665C492-8F92-431E-AB54-6825D5918930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,26 @@
     <sheet name="KHACH_HANG" sheetId="2" r:id="rId1"/>
     <sheet name="UY_QUYEN" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="203">
   <si>
     <t>HỘ KINH DOANH VẬN TẢI TIẾT KIỆM NGUYỄN THỦY</t>
   </si>
@@ -280,29 +289,371 @@
     <t>10280400235395</t>
   </si>
   <si>
-    <t>19002471660006382</t>
-  </si>
-  <si>
-    <t>19002471660006383</t>
-  </si>
-  <si>
-    <t>19002471660006384</t>
-  </si>
-  <si>
-    <t>19002471660006385</t>
-  </si>
-  <si>
-    <t>19002471660006386</t>
-  </si>
-  <si>
     <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>0947585124</t>
+  </si>
+  <si>
+    <t>phunghungk4tc@gmail.com</t>
+  </si>
+  <si>
+    <t>064092011230</t>
+  </si>
+  <si>
+    <t>Duy Tân, Thành phố Kon Tum, Kon Tum</t>
+  </si>
+  <si>
+    <t>104882125999</t>
+  </si>
+  <si>
+    <t>Viettinbank</t>
+  </si>
+  <si>
+    <t>VP P30</t>
+  </si>
+  <si>
+    <t>0933842266</t>
+  </si>
+  <si>
+    <t>001184038288</t>
+  </si>
+  <si>
+    <t>19/02/2024</t>
+  </si>
+  <si>
+    <t>Số 98 Khương Trung, Thanh Xuân, Hà Nội</t>
+  </si>
+  <si>
+    <t>VPBank</t>
+  </si>
+  <si>
+    <t>Phùng Văn Hùng</t>
+  </si>
+  <si>
+    <t>Phạm Thúy Vân</t>
+  </si>
+  <si>
+    <t>0905396696</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>049093007548</t>
+  </si>
+  <si>
+    <t>22/12/2021</t>
+  </si>
+  <si>
+    <t>176A Nguyễn Duy Hiệu, Tổ 44, An Hải Đông, Sơn Trà, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>HD Bank</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Tuấn</t>
+  </si>
+  <si>
+    <t>VP VT TK NGUYỄN THỦY 6</t>
+  </si>
+  <si>
+    <t>VP VT TK NGUYỄN THỦY 7</t>
+  </si>
+  <si>
+    <t>F1026619</t>
+  </si>
+  <si>
+    <t>F1026620</t>
+  </si>
+  <si>
+    <t>10280400756615</t>
+  </si>
+  <si>
+    <t>10280400150060</t>
+  </si>
+  <si>
+    <t>tuannh13579@gmail.com</t>
+  </si>
+  <si>
+    <t>0969795853</t>
+  </si>
+  <si>
+    <t>kien.home79@gmail.com</t>
+  </si>
+  <si>
+    <t>056099010002</t>
+  </si>
+  <si>
+    <t>04/04/2024</t>
+  </si>
+  <si>
+    <t>Thôn Tân Thủy, Ninh Lộc, Ninh Hòa, Khánh Hòa</t>
+  </si>
+  <si>
+    <t>MBBank</t>
+  </si>
+  <si>
+    <t>HỘ KINH DOANH TẠP HÓA THÁI LONG</t>
+  </si>
+  <si>
+    <t>Số 123 phố Đại La, Phường Trương Định, Quận Hai Bà Trưng, Thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t>01D8054331</t>
+  </si>
+  <si>
+    <t>Phòng Tài chính Kế hoạch Uỷ ban nhân dân Quận Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>CAO THÁI HOÀNG LONG</t>
+  </si>
+  <si>
+    <t>Xóm 2, xã Diễn An, huyện Diễn Châu, tỉnh Nghệ An</t>
+  </si>
+  <si>
+    <t>040087018136</t>
+  </si>
+  <si>
+    <t>20/08/2021</t>
+  </si>
+  <si>
+    <t>Cục Cảnh sát Quản lý hành chính về trật tư xã hội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nguyenngocminhchau140512@gmail.com </t>
+  </si>
+  <si>
+    <t>Ngày cấp ủy quyền</t>
+  </si>
+  <si>
+    <t>THÁI LONG 10</t>
+  </si>
+  <si>
+    <t>1902471660006382</t>
+  </si>
+  <si>
+    <t>1902471660006383</t>
+  </si>
+  <si>
+    <t>1902471660006384</t>
+  </si>
+  <si>
+    <t>1902471660006385</t>
+  </si>
+  <si>
+    <t>1902471660006386</t>
+  </si>
+  <si>
+    <t>1902471660006387</t>
+  </si>
+  <si>
+    <t>1902471660006388</t>
+  </si>
+  <si>
+    <t>0942673111</t>
+  </si>
+  <si>
+    <t>mrhiep686@gmail.com</t>
+  </si>
+  <si>
+    <t>038088021733</t>
+  </si>
+  <si>
+    <t>12/03/2021</t>
+  </si>
+  <si>
+    <t>Mỹ Hòa, Yên Tâm, Yên Định, Thanh Hóa</t>
+  </si>
+  <si>
+    <t>0911431988</t>
+  </si>
+  <si>
+    <t>Vietinbank</t>
+  </si>
+  <si>
+    <t>lequangcovn@gmail.com</t>
+  </si>
+  <si>
+    <t>045091003513</t>
+  </si>
+  <si>
+    <t>09/05/2021</t>
+  </si>
+  <si>
+    <t>Khu phố 2, Đông Lương, Thành phố Đông Hà, Quảng Trị</t>
+  </si>
+  <si>
+    <t>5310572493</t>
+  </si>
+  <si>
+    <t>BIDV</t>
+  </si>
+  <si>
+    <t>0949284222</t>
+  </si>
+  <si>
+    <t>Exim D210</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Kiên</t>
+  </si>
+  <si>
+    <t>Trịnh Văn Hiệp</t>
+  </si>
+  <si>
+    <t>Lê Quang Có</t>
+  </si>
+  <si>
+    <t>NGUYỄN HOÀNG TUẤN</t>
+  </si>
+  <si>
+    <t>index 10</t>
+  </si>
+  <si>
+    <t>HD X990</t>
+  </si>
+  <si>
+    <t>LÊ QUANG THIỆN</t>
+  </si>
+  <si>
+    <t>0905660999</t>
+  </si>
+  <si>
+    <t>thienle240291@gmail.com</t>
+  </si>
+  <si>
+    <t>049091003906</t>
+  </si>
+  <si>
+    <t>11/11/2021</t>
+  </si>
+  <si>
+    <t>Tổ 03, Duy Trung, Duy Xuyên, Quảng Nam</t>
+  </si>
+  <si>
+    <t>19033875971014</t>
+  </si>
+  <si>
+    <t>Techcombank</t>
+  </si>
+  <si>
+    <t>HỘ KINH DOANH VẬN TẢI VÂN TÌNH</t>
+  </si>
+  <si>
+    <t>Số 85 Dốc Ga, Phường Phú Sơn, Thành phố Thanh Hóa, Tỉnh Thanh Hóa.</t>
+  </si>
+  <si>
+    <t>26A8049403</t>
+  </si>
+  <si>
+    <t>05/08/2024</t>
+  </si>
+  <si>
+    <t>Phòng Tài chính Kế hoạch Ủy ban nhân dân Thành phố Thanh Hóa</t>
+  </si>
+  <si>
+    <t>NGUYỄN ĐÌNH TÌNH</t>
+  </si>
+  <si>
+    <t>11/38 Mật Sơn 3, Phường Đông Vệ, Thành phố Thanh Hóa, Tỉnh Thanh Hóa</t>
+  </si>
+  <si>
+    <t>85 Dốc Ga, Phường Phú Sơn, Thành phố Thanh Hóa, Tỉnh Thanh Hóa</t>
+  </si>
+  <si>
+    <t>038090001357</t>
+  </si>
+  <si>
+    <t>22/06/2022</t>
+  </si>
+  <si>
+    <t>HỘ KINH DOANH VẬN TẢI NGUYỄN VĂN SỬ</t>
+  </si>
+  <si>
+    <t>Số 34, ngách 15, Ngõ 14 Phương Mai, Phường Phương Mai, Quận Đống Đa, Thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t>01E8040746</t>
+  </si>
+  <si>
+    <t>13/05/2024</t>
+  </si>
+  <si>
+    <t>Phòng tài chính kế hoạch Ủy ban nhân dân quận Đống Đa</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN SỬ</t>
+  </si>
+  <si>
+    <t>Khu 4, Xã Phùng Nguyên, Huyện Lâm Thao, Tỉnh Phú Thọ</t>
+  </si>
+  <si>
+    <t>025092007614</t>
+  </si>
+  <si>
+    <t>08/12/2021</t>
+  </si>
+  <si>
+    <t>Phan Hoàng Hải</t>
+  </si>
+  <si>
+    <t>0934789789</t>
+  </si>
+  <si>
+    <t>hoanghai.phan@gmail.com</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>13/07/2000</t>
+  </si>
+  <si>
+    <t>111 Đống Đa, Thạch Thang, Hải Châu, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>01111111111111</t>
+  </si>
+  <si>
+    <t>0905123456</t>
+  </si>
+  <si>
+    <t>phanhoanghai@gmail.com</t>
+  </si>
+  <si>
+    <t>00987654321</t>
+  </si>
+  <si>
+    <t>13/07/2010</t>
+  </si>
+  <si>
+    <t>222 Lý Tự Trọng, Thạch Thang, Hải Châu, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>02222</t>
+  </si>
+  <si>
+    <t>HUỲNH VĂN HUY</t>
+  </si>
+  <si>
+    <t>dia_chi_giao_hang</t>
+  </si>
+  <si>
+    <t>dc_giao_hang</t>
+  </si>
+  <si>
+    <t>PHAN HOÀNG HẢI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,13 +669,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -336,10 +713,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -359,8 +737,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,34 +1033,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCE07E-0643-476E-9C29-D6F951414B39}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="43.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.6640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="18.21875" style="5" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="4.0"/>
+    <col min="2" max="2" customWidth="true" style="1" width="20.44140625"/>
+    <col min="3" max="3" customWidth="true" style="5" width="12.44140625"/>
+    <col min="4" max="4" customWidth="true" style="1" width="26.44140625"/>
+    <col min="5" max="5" customWidth="true" style="5" width="14.33203125"/>
+    <col min="6" max="6" customWidth="true" style="5" width="11.77734375"/>
+    <col min="7" max="7" customWidth="true" style="1" width="18.5546875"/>
+    <col min="8" max="8" customWidth="true" style="1" width="43.21875"/>
+    <col min="9" max="9" customWidth="true" style="5" width="15.33203125"/>
+    <col min="10" max="10" customWidth="true" style="1" width="13.6640625"/>
+    <col min="11" max="11" customWidth="true" style="1" width="16.109375"/>
+    <col min="12" max="12" customWidth="true" style="1" width="12.44140625"/>
+    <col min="13" max="13" customWidth="true" style="1" width="26.33203125"/>
+    <col min="14" max="14" customWidth="true" style="5" width="21.6640625"/>
+    <col min="15" max="15" customWidth="true" style="5" width="19.21875"/>
+    <col min="16" max="16" customWidth="true" style="1" width="12.6640625"/>
+    <col min="17" max="17" customWidth="true" style="11" width="11.6640625"/>
+    <col min="18" max="16384" style="1" width="8.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -674,7 +1069,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>28</v>
@@ -715,8 +1110,11 @@
       <c r="P1" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -754,7 +1152,7 @@
         <v>41</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>79</v>
@@ -762,8 +1160,11 @@
       <c r="P2" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" s="11">
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -801,7 +1202,7 @@
         <v>47</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>80</v>
@@ -809,8 +1210,11 @@
       <c r="P3" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="11">
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -848,7 +1252,7 @@
         <v>49</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>81</v>
@@ -856,8 +1260,11 @@
       <c r="P4" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="11">
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -895,7 +1302,7 @@
         <v>56</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>82</v>
@@ -903,8 +1310,11 @@
       <c r="P5" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5" s="11">
+        <v>45580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -942,7 +1352,7 @@
         <v>63</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>83</v>
@@ -950,35 +1360,695 @@
       <c r="P6" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="Q6" s="11">
+        <v>45580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>45586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>45586</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>45589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s" s="1">
+        <v>199</v>
+      </c>
+      <c r="C18" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s" s="5">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="I18" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="J18" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="K18" t="s" s="1">
+        <v>200</v>
+      </c>
+      <c r="L18" t="s" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n" s="2">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s" s="1">
+        <v>199</v>
+      </c>
+      <c r="C19" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s" s="5">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="H19" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="I19" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="J19" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="K19" t="s" s="1">
+        <v>200</v>
+      </c>
+      <c r="L19" t="s" s="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="2">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s" s="1">
+        <v>199</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s" s="5">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="H20" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="I20" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="J20" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="K20" t="s" s="1">
+        <v>200</v>
+      </c>
+      <c r="L20" t="s" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s" s="1">
+        <v>199</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s" s="5">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="H21" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="I21" t="s" s="5">
+        <v>68</v>
+      </c>
+      <c r="J21" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="K21" t="s" s="1">
+        <v>201</v>
+      </c>
+      <c r="L21" t="s" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s" s="1">
+        <v>202</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>193</v>
+      </c>
+      <c r="D22" t="s" s="1">
+        <v>194</v>
+      </c>
+      <c r="E22" t="s" s="5">
+        <v>195</v>
+      </c>
+      <c r="F22" t="s" s="5">
+        <v>196</v>
+      </c>
+      <c r="G22" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s" s="1">
+        <v>197</v>
+      </c>
+      <c r="I22" t="s" s="5">
+        <v>198</v>
+      </c>
+      <c r="J22" t="s" s="1">
+        <v>166</v>
+      </c>
+      <c r="K22" t="s" s="1">
+        <v>201</v>
+      </c>
+      <c r="L22" t="s" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="2">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s" s="1">
+        <v>202</v>
+      </c>
+      <c r="C23" t="s" s="5">
+        <v>193</v>
+      </c>
+      <c r="D23" t="s" s="1">
+        <v>194</v>
+      </c>
+      <c r="E23" t="s" s="5">
+        <v>195</v>
+      </c>
+      <c r="F23" t="s" s="5">
+        <v>196</v>
+      </c>
+      <c r="G23" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s" s="1">
+        <v>197</v>
+      </c>
+      <c r="I23" t="s" s="5">
+        <v>198</v>
+      </c>
+      <c r="J23" t="s" s="1">
+        <v>166</v>
+      </c>
+      <c r="K23" t="s" s="1">
+        <v>201</v>
+      </c>
+      <c r="L23" t="s" s="1">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{ED497DD7-CA75-46EA-9200-43E1BEAF36B4}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{E43C4636-D605-49CC-B87B-5320492185DC}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{2BF8BB07-19D8-4849-9E6F-EBA31F0F7E51}"/>
+    <hyperlink ref="D17" r:id="rId4" xr:uid="{7146AF2E-B915-4E37-8C56-C65D66D38967}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="4.0"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.109375"/>
+    <col min="3" max="3" customWidth="true" style="1" width="25.5546875"/>
+    <col min="4" max="4" customWidth="true" style="1" width="12.44140625"/>
+    <col min="5" max="5" customWidth="true" style="1" width="11.44140625"/>
+    <col min="6" max="6" customWidth="true" style="1" width="19.21875"/>
+    <col min="7" max="7" customWidth="true" style="1" width="13.5546875"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.21875"/>
+    <col min="9" max="9" customWidth="true" style="1" width="27.5546875"/>
+    <col min="10" max="10" customWidth="true" style="5" width="12.88671875"/>
+    <col min="11" max="11" customWidth="true" style="1" width="11.33203125"/>
+    <col min="12" max="12" customWidth="true" style="1" width="15.6640625"/>
+    <col min="13" max="16384" style="1" width="8.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1095,6 +2165,120 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finalize app version 3.0
</commit_message>
<xml_diff>
--- a/sourceDocs/THONG_TIN.xlsx
+++ b/sourceDocs/THONG_TIN.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAIPH\Downloads\sourceDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAIPH\Downloads\HO_SO_POS V2.0\sourceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58A97C6-CBF2-4545-A57D-A518A0BB7ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065ACAAB-0A9D-4331-B6FE-1CAC8938CD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KHACH_HANG" sheetId="2" r:id="rId1"/>
@@ -18,24 +18,15 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="292">
   <si>
     <t>HỘ KINH DOANH VẬN TẢI TIẾT KIỆM NGUYỄN THỦY</t>
   </si>
@@ -491,6 +482,426 @@
   </si>
   <si>
     <t>Số lượng</t>
+  </si>
+  <si>
+    <t>LƯU TIỂU HẠNH</t>
+  </si>
+  <si>
+    <t>0905963964</t>
+  </si>
+  <si>
+    <t>hanhluu169@gmail.com</t>
+  </si>
+  <si>
+    <t>279186000001</t>
+  </si>
+  <si>
+    <t>Tổ 23, Thanh Khê Tây, Thanh Khê, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>19025419282018</t>
+  </si>
+  <si>
+    <t>dc_giao_hang</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>NGUYỄN ĐỨC NHUẬN</t>
+  </si>
+  <si>
+    <t>0792692279</t>
+  </si>
+  <si>
+    <t>nguyennhuan2110@gmail.com</t>
+  </si>
+  <si>
+    <t>056094005775</t>
+  </si>
+  <si>
+    <t>14/01/2022</t>
+  </si>
+  <si>
+    <t>Thôn Lạc An, Ninh Thọ, Thị xã Ninh Hòa, Khánh Hòa</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TRƯƠNG THỊ THU HÀ</t>
+  </si>
+  <si>
+    <t>0936223505</t>
+  </si>
+  <si>
+    <t>nguỹenuandong90@gmail.com</t>
+  </si>
+  <si>
+    <t>077190007713</t>
+  </si>
+  <si>
+    <t>09/01/2022</t>
+  </si>
+  <si>
+    <t>Ấp 1 Bầu Lâm, Xuyên Mộc, Bà Rịa - Vũng Tàu</t>
+  </si>
+  <si>
+    <t>TRẦN THỊ HOÀNG LY</t>
+  </si>
+  <si>
+    <t>0799345489</t>
+  </si>
+  <si>
+    <t>hoanglybds@gmail.com</t>
+  </si>
+  <si>
+    <t>048190006314</t>
+  </si>
+  <si>
+    <t>Tổ 24, An Hải Bắc, Sơn Trà, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>VŨ TIẾN MẠNH</t>
+  </si>
+  <si>
+    <t>0392225789</t>
+  </si>
+  <si>
+    <t>vutienmanhvtv8@gmail.com</t>
+  </si>
+  <si>
+    <t>001079024270</t>
+  </si>
+  <si>
+    <t>05/11/2022</t>
+  </si>
+  <si>
+    <t>603-17T2 Hapulico, 1 Nguyễn Huy Tưởng, Thanh Xuân Trung, Thanh Xuân, Hà Nội</t>
+  </si>
+  <si>
+    <t>Eximbank</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>HỘ KINH DOANH VẬN TẢI LUẬN HOA</t>
+  </si>
+  <si>
+    <t>Số 17A ngõ 124 Nguyễn Xiển, Phường Hạ Đình, Quận Thanh Xuân, Thành Phố Hà Nội</t>
+  </si>
+  <si>
+    <t>01F8025835</t>
+  </si>
+  <si>
+    <t>27/05/2024</t>
+  </si>
+  <si>
+    <t>Phòng tài chính kế hoạch Ủy ban nhân dân Quận Thanh Xuân</t>
+  </si>
+  <si>
+    <t>NGUYỄN CÔNG LUẬN</t>
+  </si>
+  <si>
+    <t>Thôn 3 An Định, Xã Thụy Văn, Huyện Thái Thụy, Tỉnh Thái Bình</t>
+  </si>
+  <si>
+    <t>034089007984</t>
+  </si>
+  <si>
+    <t>08/01/2024</t>
+  </si>
+  <si>
+    <t>HỘ KINH DOANH VẬN TẢI VĂN DƯƠNG</t>
+  </si>
+  <si>
+    <t>Số nhà 12 ngõ 102 đường Khuất Duy Tiến, Phường Nhân Chính, Quận Thanh Xuân, Thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t>01F8026330</t>
+  </si>
+  <si>
+    <t>25/07/2024</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN DƯƠNG</t>
+  </si>
+  <si>
+    <t>Phố Thiều, Xã Dân Lý, Huyện Triệu Sơn, Tỉnh Thanh Hóa</t>
+  </si>
+  <si>
+    <t>038098005431</t>
+  </si>
+  <si>
+    <t>26/05/2023</t>
+  </si>
+  <si>
+    <t>nguyenxuandong90@gmail.com</t>
+  </si>
+  <si>
+    <t>19037197662011</t>
+  </si>
+  <si>
+    <t>LÊ VĂN QUANG</t>
+  </si>
+  <si>
+    <t>0931122102</t>
+  </si>
+  <si>
+    <t>Lequangqn89@gmail.com</t>
+  </si>
+  <si>
+    <t>049089006723</t>
+  </si>
+  <si>
+    <t>28/06/2021</t>
+  </si>
+  <si>
+    <t>K04/H2/2 Đặng Thùy Trâm, Hải Châu, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>VƯƠNG THỊ HẢI</t>
+  </si>
+  <si>
+    <t>0847117117</t>
+  </si>
+  <si>
+    <t>danangtindung@gmail.com</t>
+  </si>
+  <si>
+    <t>038186033214</t>
+  </si>
+  <si>
+    <t>29/01/2023</t>
+  </si>
+  <si>
+    <t>Tổ 19, Hòa Khánh Nam, Liên Chiểu, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>968279968</t>
+  </si>
+  <si>
+    <t>HUỲNH THANH TÂM</t>
+  </si>
+  <si>
+    <t>0943727374</t>
+  </si>
+  <si>
+    <t>kcstam@gmail.com</t>
+  </si>
+  <si>
+    <t>060086004622</t>
+  </si>
+  <si>
+    <t>27/08/2022</t>
+  </si>
+  <si>
+    <t>Tổ 7, Khu phố 9, Mũi Né, TP. Phan Thiết, Bình Thuận</t>
+  </si>
+  <si>
+    <t>3979727374</t>
+  </si>
+  <si>
+    <t>HUỲNH VĂN HUY</t>
+  </si>
+  <si>
+    <t>NGUYỄN PHƯƠNG THÚY</t>
+  </si>
+  <si>
+    <t>0988851816</t>
+  </si>
+  <si>
+    <t>Thuy.lak94@gmail.com</t>
+  </si>
+  <si>
+    <t>040195005288</t>
+  </si>
+  <si>
+    <t>27/04/2021</t>
+  </si>
+  <si>
+    <t>Khối 6, Cửa Nam, Thành phố Vinh, Tỉnh Nghệ An</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>LÊ THỊ NGỌC HIẾU</t>
+  </si>
+  <si>
+    <t>VP X990</t>
+  </si>
+  <si>
+    <t>PHÙNG VĂN HÙNG</t>
+  </si>
+  <si>
+    <t>HUỲNH HỮU HẠN</t>
+  </si>
+  <si>
+    <t>0966410011</t>
+  </si>
+  <si>
+    <t>huuhan560422@gmail.com</t>
+  </si>
+  <si>
+    <t>056079000543</t>
+  </si>
+  <si>
+    <t>08/04/2021</t>
+  </si>
+  <si>
+    <t>16 Đường 23/10, Phương Sơn, Nha Trang, Khánh Hòa</t>
+  </si>
+  <si>
+    <t>LÊ THỊ DIỆU HIỀN</t>
+  </si>
+  <si>
+    <t>0963313933</t>
+  </si>
+  <si>
+    <t>lehien170993@gmail.com</t>
+  </si>
+  <si>
+    <t>064193002452</t>
+  </si>
+  <si>
+    <t>Tổ 3, Hội Thương, Thành phố Pleiku, Gia Lai</t>
+  </si>
+  <si>
+    <t>08959686</t>
+  </si>
+  <si>
+    <t>MB Bank</t>
+  </si>
+  <si>
+    <t>LÊ QUANG CÓ</t>
+  </si>
+  <si>
+    <t>Ngân hàng Eximbank</t>
+  </si>
+  <si>
+    <t>ĐÀO ANH VIỆT</t>
+  </si>
+  <si>
+    <t>PHAN THANH ĐẠI</t>
+  </si>
+  <si>
+    <t>0868134747</t>
+  </si>
+  <si>
+    <t>monstermax0007@gmail.com</t>
+  </si>
+  <si>
+    <t>066096019550</t>
+  </si>
+  <si>
+    <t>10/03/2023</t>
+  </si>
+  <si>
+    <t>Thôn 3 Ea Kao, Buôn Ma Thuột, Đắk Lắk</t>
+  </si>
+  <si>
+    <t>0231000668635</t>
+  </si>
+  <si>
+    <t>Ngân hàng Vietcombank</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>MST</t>
+  </si>
+  <si>
+    <t>Tên cửa hàng</t>
+  </si>
+  <si>
+    <t>PHAN HUY HOÀNG</t>
+  </si>
+  <si>
+    <t>08/03/1995</t>
+  </si>
+  <si>
+    <t>0935003445</t>
+  </si>
+  <si>
+    <t>huyhoang.phan@gmail.com</t>
+  </si>
+  <si>
+    <t>048095000369</t>
+  </si>
+  <si>
+    <t>160/63 Trần Cao Vân, Phường Tam Thuận, Quận Thanh Khê, Thành phố Đà Nẵng</t>
+  </si>
+  <si>
+    <t>1199399699</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>TẬP ĐOÀN PHAN THỊ</t>
+  </si>
+  <si>
+    <t>111 Nguyễn Du, Phường Thạch Thang, Quận Hải Châu, Thành phố Đà Nẵng</t>
+  </si>
+  <si>
+    <t>9D9999999</t>
+  </si>
+  <si>
+    <t>15/10/2020</t>
+  </si>
+  <si>
+    <t>Phòng Tài chính Kế hoạch Quận Hải Châu</t>
+  </si>
+  <si>
+    <t>6868686868</t>
+  </si>
+  <si>
+    <t>phan thị</t>
+  </si>
+  <si>
+    <t>PHAN HOÀNG HẢI</t>
+  </si>
+  <si>
+    <t>201585869</t>
+  </si>
+  <si>
+    <t>13/07/2010</t>
+  </si>
+  <si>
+    <t>Công an Đà Nẵng</t>
+  </si>
+  <si>
+    <t>0989898989</t>
+  </si>
+  <si>
+    <t>haiph@phanthi.com</t>
+  </si>
+  <si>
+    <t>07/03/1997</t>
+  </si>
+  <si>
+    <t>0935003456</t>
+  </si>
+  <si>
+    <t>huyhoang.phan1@gmail.com</t>
+  </si>
+  <si>
+    <t>048095000378</t>
+  </si>
+  <si>
+    <t>111 Trần Cao Vân, Phường Tam Thuận, Quận Thanh Khê, Thành phố Đà Nẵng</t>
+  </si>
+  <si>
+    <t>1199399600</t>
   </si>
 </sst>
 </file>
@@ -865,591 +1276,1714 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCE07E-0643-476E-9C29-D6F951414B39}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="4.0"/>
+    <col min="2" max="2" customWidth="true" style="1" width="23.5546875"/>
+    <col min="3" max="3" customWidth="true" style="1" width="17.33203125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="9" width="12.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="24.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="9" width="13.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="9" width="10.5546875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="18.21875"/>
+    <col min="9" max="9" customWidth="true" style="1" width="39.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="9" width="15.109375"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="12.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="15.44140625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="9.5546875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="8.6640625"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="8" width="17.33203125"/>
+    <col min="16" max="16384" style="1" width="8.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="8">
+      <c r="O2" s="8">
         <v>45579</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="8">
+      <c r="O3" s="8">
         <v>45579</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="8">
+      <c r="O4" s="8">
         <v>45579</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="8">
+      <c r="O5" s="8">
         <v>45580</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="8">
+      <c r="O6" s="8">
         <v>45580</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="8">
+      <c r="O7" s="8">
         <v>45586</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N8" s="8">
+      <c r="O8" s="8">
         <v>45586</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N10" s="8">
+      <c r="O10" s="8">
         <v>45589</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="J13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="J14" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="J15" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="2">
+        <v>38.0</v>
+      </c>
+      <c r="B39" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C39" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="D39" t="s" s="9">
+        <v>265</v>
+      </c>
+      <c r="E39" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="F39" t="s" s="9">
+        <v>267</v>
+      </c>
+      <c r="G39" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="H39" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I39" t="s" s="1">
+        <v>268</v>
+      </c>
+      <c r="J39" t="s" s="9">
+        <v>269</v>
+      </c>
+      <c r="K39" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L39" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="2">
+        <v>39.0</v>
+      </c>
+      <c r="B40" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C40" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="D40" t="s" s="9">
+        <v>265</v>
+      </c>
+      <c r="E40" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="F40" t="s" s="9">
+        <v>267</v>
+      </c>
+      <c r="G40" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="H40" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I40" t="s" s="1">
+        <v>268</v>
+      </c>
+      <c r="J40" t="s" s="9">
+        <v>269</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L40" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="B41" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C41" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="D41" t="s" s="9">
+        <v>265</v>
+      </c>
+      <c r="E41" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="F41" t="s" s="9">
+        <v>267</v>
+      </c>
+      <c r="G41" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="H41" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I41" t="s" s="1">
+        <v>268</v>
+      </c>
+      <c r="J41" t="s" s="9">
+        <v>269</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L41" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="2">
+        <v>41.0</v>
+      </c>
+      <c r="B42" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C42" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="D42" t="s" s="9">
+        <v>287</v>
+      </c>
+      <c r="E42" t="s" s="1">
+        <v>288</v>
+      </c>
+      <c r="F42" t="s" s="9">
+        <v>289</v>
+      </c>
+      <c r="G42" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="H42" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I42" t="s" s="1">
+        <v>290</v>
+      </c>
+      <c r="J42" t="s" s="9">
+        <v>291</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L42" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" xr:uid="{ED497DD7-CA75-46EA-9200-43E1BEAF36B4}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{E43C4636-D605-49CC-B87B-5320492185DC}"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{ED497DD7-CA75-46EA-9200-43E1BEAF36B4}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{E43C4636-D605-49CC-B87B-5320492185DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -1458,31 +2992,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="4.0"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.33203125"/>
+    <col min="3" max="3" customWidth="true" style="1" width="25.5546875"/>
+    <col min="4" max="4" customWidth="true" style="1" width="12.44140625"/>
+    <col min="5" max="5" customWidth="true" style="1" width="11.44140625"/>
+    <col min="6" max="6" customWidth="true" style="1" width="21.21875"/>
+    <col min="7" max="7" customWidth="true" style="1" width="16.6640625"/>
+    <col min="8" max="8" customWidth="true" style="1" width="20.21875"/>
+    <col min="9" max="9" customWidth="true" style="1" width="13.5546875"/>
+    <col min="10" max="10" customWidth="true" style="1" width="26.21875"/>
+    <col min="11" max="11" customWidth="true" style="1" width="27.5546875"/>
+    <col min="12" max="12" customWidth="true" style="5" width="12.88671875"/>
+    <col min="13" max="13" customWidth="true" style="1" width="11.33203125"/>
+    <col min="14" max="14" customWidth="true" style="1" width="15.6640625"/>
+    <col min="15" max="15" customWidth="true" style="1" width="15.33203125"/>
+    <col min="16" max="16384" style="1" width="8.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1502,25 +3038,37 @@
         <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1539,26 +3087,26 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="5">
+      <c r="L2" s="5">
         <v>38185003810</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1577,26 +3125,26 @@
       <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1615,26 +3163,26 @@
       <c r="F4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1653,26 +3201,26 @@
       <c r="F5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1691,27 +3239,154 @@
       <c r="F6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="6"/>
+      <c r="N6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s" s="1">
+        <v>273</v>
+      </c>
+      <c r="C9" t="s" s="1">
+        <v>274</v>
+      </c>
+      <c r="D9" t="s" s="1">
+        <v>275</v>
+      </c>
+      <c r="E9" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="F9" t="s" s="1">
+        <v>277</v>
+      </c>
+      <c r="G9" t="s" s="1">
+        <v>278</v>
+      </c>
+      <c r="H9" t="s" s="1">
+        <v>279</v>
+      </c>
+      <c r="I9" t="s" s="1">
+        <v>280</v>
+      </c>
+      <c r="J9" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="K9" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="L9" t="s" s="5">
+        <v>281</v>
+      </c>
+      <c r="M9" t="s" s="1">
+        <v>282</v>
+      </c>
+      <c r="N9" t="s" s="1">
+        <v>283</v>
+      </c>
+      <c r="O9" t="s" s="1">
+        <v>284</v>
+      </c>
+      <c r="P9" t="s" s="1">
+        <v>285</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
release app version 4.0
</commit_message>
<xml_diff>
--- a/sourceDocs/THONG_TIN.xlsx
+++ b/sourceDocs/THONG_TIN.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAIPH\Downloads\HO_SO_POS V2.0\sourceDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\testProject\auto-complete-docx-form\sourceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065ACAAB-0A9D-4331-B6FE-1CAC8938CD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C23DDE3-44B4-40D7-921B-477BE4EFB833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KHACH_HANG" sheetId="2" r:id="rId1"/>
     <sheet name="UY_QUYEN" sheetId="1" r:id="rId2"/>
+    <sheet name="NHAN_VIEN" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="338">
   <si>
     <t>HỘ KINH DOANH VẬN TẢI TIẾT KIỆM NGUYỄN THỦY</t>
   </si>
@@ -865,9 +866,6 @@
     <t>6868686868</t>
   </si>
   <si>
-    <t>phan thị</t>
-  </si>
-  <si>
     <t>PHAN HOÀNG HẢI</t>
   </si>
   <si>
@@ -902,6 +900,147 @@
   </si>
   <si>
     <t>1199399600</t>
+  </si>
+  <si>
+    <t>Tên nhân viên</t>
+  </si>
+  <si>
+    <t>NGUYỄN THỊ HOÀNG YẾN</t>
+  </si>
+  <si>
+    <t>042193017175</t>
+  </si>
+  <si>
+    <t>Số hợp đồng</t>
+  </si>
+  <si>
+    <t>0999</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>212 Lol</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>123321456</t>
+  </si>
+  <si>
+    <t>HẢI</t>
+  </si>
+  <si>
+    <t>0123</t>
+  </si>
+  <si>
+    <t>lol@gmail.com</t>
+  </si>
+  <si>
+    <t>TEST2</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>TEST22</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>7777</t>
+  </si>
+  <si>
+    <t>TẬP ĐOÀN PHAN PHAN</t>
+  </si>
+  <si>
+    <t>01357</t>
+  </si>
+  <si>
+    <t>6666</t>
+  </si>
+  <si>
+    <t>PHAN ANH QUÂN</t>
+  </si>
+  <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
+    <t>0123456765</t>
+  </si>
+  <si>
+    <t>123312</t>
+  </si>
+  <si>
+    <t>2222222222</t>
+  </si>
+  <si>
+    <t>123321</t>
+  </si>
+  <si>
+    <t>1111111</t>
+  </si>
+  <si>
+    <t>111111111</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH ĐÀU TƯ VÀ XÂY DỰNG NGUYÊN LÂM</t>
+  </si>
+  <si>
+    <t>123 Thanh Thủy, Phường Thuận Phước, Quận Hải Châu, TP Đà Nẵng</t>
+  </si>
+  <si>
+    <t>123TEST321</t>
+  </si>
+  <si>
+    <t>13/10/2010</t>
+  </si>
+  <si>
+    <t>Phòng tài chính kế hoạch Quận Hải Châu</t>
+  </si>
+  <si>
+    <t>PHAN THANH SƠN</t>
+  </si>
+  <si>
+    <t>0411123456</t>
+  </si>
+  <si>
+    <t>13/10/2021</t>
+  </si>
+  <si>
+    <t>0911111111</t>
+  </si>
+  <si>
+    <t>son.pt@nguyenlam.com</t>
+  </si>
+  <si>
+    <t>NGUYÊN LÂM 12</t>
+  </si>
+  <si>
+    <t>201585870</t>
+  </si>
+  <si>
+    <t>PHAN THỊ</t>
+  </si>
+  <si>
+    <t>PHAN HOÀNG QUÂN</t>
+  </si>
+  <si>
+    <t>201585871</t>
+  </si>
+  <si>
+    <t>13/07/2021</t>
+  </si>
+  <si>
+    <t>Đà Nẵng</t>
+  </si>
+  <si>
+    <t>38185003810</t>
+  </si>
+  <si>
+    <t>045183000800</t>
   </si>
 </sst>
 </file>
@@ -963,7 +1102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -995,6 +1134,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1276,7 +1416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCE07E-0643-476E-9C29-D6F951414B39}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -2803,180 +2943,646 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="n" s="2">
-        <v>38.0</v>
-      </c>
-      <c r="B39" t="s" s="1">
+    <row r="39" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C39" t="s" s="1">
+      <c r="C39" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D39" t="s" s="9">
+      <c r="D39" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="E39" t="s" s="1">
+      <c r="E39" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F39" t="s" s="9">
+      <c r="F39" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="G39" t="s" s="9">
+      <c r="G39" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H39" t="s" s="1">
-        <v>8</v>
-      </c>
-      <c r="I39" t="s" s="1">
+      <c r="H39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J39" t="s" s="9">
+      <c r="J39" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="K39" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="L39" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="M39" t="s" s="2">
+      <c r="L39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M39" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="N39" t="s" s="2">
+      <c r="N39" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="n" s="2">
-        <v>39.0</v>
-      </c>
-      <c r="B40" t="s" s="1">
+    <row r="40" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C40" t="s" s="1">
+      <c r="C40" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D40" t="s" s="9">
+      <c r="D40" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="E40" t="s" s="1">
+      <c r="E40" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F40" t="s" s="9">
+      <c r="F40" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="G40" t="s" s="9">
+      <c r="G40" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H40" t="s" s="1">
-        <v>8</v>
-      </c>
-      <c r="I40" t="s" s="1">
+      <c r="H40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J40" t="s" s="9">
+      <c r="J40" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="K40" t="s" s="2">
+      <c r="K40" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="L40" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="M40" t="s" s="2">
+      <c r="L40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M40" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="N40" t="s" s="2">
+      <c r="N40" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="n" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="B41" t="s" s="1">
+    <row r="41" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C41" t="s" s="1">
+      <c r="C41" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D41" t="s" s="9">
+      <c r="D41" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="E41" t="s" s="1">
+      <c r="E41" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F41" t="s" s="9">
+      <c r="F41" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="G41" t="s" s="9">
+      <c r="G41" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H41" t="s" s="1">
-        <v>8</v>
-      </c>
-      <c r="I41" t="s" s="1">
+      <c r="H41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J41" t="s" s="9">
+      <c r="J41" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="K41" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="L41" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="M41" t="s" s="2">
+      <c r="L41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M41" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N41" t="s" s="2">
+      <c r="N41" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="n" s="2">
-        <v>41.0</v>
-      </c>
-      <c r="B42" t="s" s="1">
+    <row r="42" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C42" t="s" s="1">
+      <c r="C42" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="D42" t="s" s="9">
+      <c r="E42" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E42" t="s" s="1">
+      <c r="F42" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F42" t="s" s="9">
+      <c r="G42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G42" t="s" s="9">
+      <c r="J42" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H42" t="s" s="1">
-        <v>8</v>
-      </c>
-      <c r="I42" t="s" s="1">
-        <v>290</v>
-      </c>
-      <c r="J42" t="s" s="9">
-        <v>291</v>
-      </c>
-      <c r="K42" t="s" s="2">
+      <c r="H43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="L42" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="M42" t="s" s="2">
+      <c r="L43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N42" t="s" s="2">
+      <c r="N45" s="2" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2992,10 +3598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3015,10 +3621,12 @@
     <col min="13" max="13" customWidth="true" style="1" width="11.33203125"/>
     <col min="14" max="14" customWidth="true" style="1" width="15.6640625"/>
     <col min="15" max="15" customWidth="true" style="1" width="15.33203125"/>
-    <col min="16" max="16384" style="1" width="8.88671875"/>
+    <col min="16" max="16" style="1" width="8.88671875"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="5" width="11.77734375"/>
+    <col min="18" max="16384" style="1" width="8.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -3067,8 +3675,11 @@
       <c r="P1" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q1" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3087,17 +3698,23 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G2" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="H2" t="s" s="1">
+        <v>81</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="5">
-        <v>38185003810</v>
+        <v>81</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>336</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>7</v>
@@ -3105,8 +3722,17 @@
       <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O2" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="P2" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="Q2" t="s" s="5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3125,17 +3751,23 @@
       <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="G3" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="H3" t="s" s="1">
+        <v>81</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>25</v>
+        <v>337</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>26</v>
@@ -3143,8 +3775,17 @@
       <c r="N3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O3" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="P3" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="Q3" t="s" s="5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3182,7 +3823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3220,7 +3861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3259,7 +3900,7 @@
       </c>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3297,7 +3938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3335,58 +3976,415 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="B9" t="s" s="1">
+    <row r="9" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C9" t="s" s="1">
+      <c r="C9" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D9" t="s" s="1">
+      <c r="D9" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E9" t="s" s="1">
+      <c r="E9" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="F9" t="s" s="1">
+      <c r="F9" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G9" t="s" s="1">
+      <c r="G9" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="H9" t="s" s="1">
+      <c r="H9" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I9" t="s" s="1">
+      <c r="J9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="J9" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="K9" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="L9" t="s" s="5">
+      <c r="M9" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="M9" t="s" s="1">
+      <c r="N9" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="N9" t="s" s="1">
+      <c r="O9" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="O9" t="s" s="1">
+      <c r="P9" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="P9" t="s" s="1">
-        <v>285</v>
+      <c r="Q9" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7781E2F-2DFA-453F-A75E-FD8E0765D7A9}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="26.5546875"/>
+    <col min="3" max="3" customWidth="true" style="11" width="18.5546875"/>
+    <col min="4" max="4" customWidth="true" style="11" width="15.5546875"/>
+    <col min="5" max="5" customWidth="true" width="31.44140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>279</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>332</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
release app version 5.0
</commit_message>
<xml_diff>
--- a/sourceDocs/THONG_TIN.xlsx
+++ b/sourceDocs/THONG_TIN.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="339">
   <si>
     <t>HỘ KINH DOANH VẬN TẢI TIẾT KIỆM NGUYỄN THỦY</t>
   </si>
@@ -1041,6 +1041,9 @@
   </si>
   <si>
     <t>045183000800</t>
+  </si>
+  <si>
+    <t>TRẦN VĂN VƯƠNG</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCE07E-0643-476E-9C29-D6F951414B39}">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -3582,6 +3585,234 @@
         <v>248</v>
       </c>
       <c r="L53" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n" s="2">
+        <v>53.0</v>
+      </c>
+      <c r="B54" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C54" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="D54" t="s" s="9">
+        <v>265</v>
+      </c>
+      <c r="E54" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="F54" t="s" s="9">
+        <v>267</v>
+      </c>
+      <c r="G54" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="H54" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I54" t="s" s="1">
+        <v>268</v>
+      </c>
+      <c r="J54" t="s" s="9">
+        <v>269</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L54" t="s" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n" s="2">
+        <v>54.0</v>
+      </c>
+      <c r="B55" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="C55" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="D55" t="s" s="9">
+        <v>253</v>
+      </c>
+      <c r="E55" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="F55" t="s" s="9">
+        <v>255</v>
+      </c>
+      <c r="G55" t="s" s="9">
+        <v>256</v>
+      </c>
+      <c r="H55" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I55" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="J55" t="s" s="9">
+        <v>258</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="L55" t="s" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="B56" t="s" s="1">
+        <v>338</v>
+      </c>
+      <c r="C56" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="D56" t="s" s="9">
+        <v>53</v>
+      </c>
+      <c r="E56" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="F56" t="s" s="9">
+        <v>57</v>
+      </c>
+      <c r="G56" t="s" s="9">
+        <v>61</v>
+      </c>
+      <c r="H56" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="I56" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="J56" t="s" s="9">
+        <v>53</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="L56" t="s" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n" s="2">
+        <v>56.0</v>
+      </c>
+      <c r="B57" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C57" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="D57" t="s" s="9">
+        <v>265</v>
+      </c>
+      <c r="E57" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="F57" t="s" s="9">
+        <v>267</v>
+      </c>
+      <c r="G57" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="H57" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I57" t="s" s="1">
+        <v>268</v>
+      </c>
+      <c r="J57" t="s" s="9">
+        <v>269</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L57" t="s" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n" s="2">
+        <v>57.0</v>
+      </c>
+      <c r="B58" t="s" s="1">
+        <v>173</v>
+      </c>
+      <c r="C58" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="D58" t="s" s="9">
+        <v>174</v>
+      </c>
+      <c r="E58" t="s" s="1">
+        <v>175</v>
+      </c>
+      <c r="F58" t="s" s="9">
+        <v>176</v>
+      </c>
+      <c r="G58" t="s" s="9">
+        <v>128</v>
+      </c>
+      <c r="H58" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="I58" t="s" s="1">
+        <v>177</v>
+      </c>
+      <c r="J58" t="s" s="9">
+        <v>81</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L58" t="s" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n" s="2">
+        <v>58.0</v>
+      </c>
+      <c r="B59" t="s" s="1">
+        <v>338</v>
+      </c>
+      <c r="C59" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="D59" t="s" s="9">
+        <v>53</v>
+      </c>
+      <c r="E59" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="F59" t="s" s="9">
+        <v>57</v>
+      </c>
+      <c r="G59" t="s" s="9">
+        <v>61</v>
+      </c>
+      <c r="H59" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="I59" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="J59" t="s" s="9">
+        <v>53</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="L59" t="s" s="1">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update: - source docs - export function
</commit_message>
<xml_diff>
--- a/sourceDocs/THONG_TIN.xlsx
+++ b/sourceDocs/THONG_TIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\testProject\auto-complete-docx-form\sourceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92BF67E-1A95-46AD-AB8F-DDBE41F3E739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F21A70F-2474-4113-8B7E-21CCD0F194D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="350">
   <si>
     <t>HỘ KINH DOANH VẬN TẢI TIẾT KIỆM NGUYỄN THỦY</t>
   </si>
@@ -1073,67 +1073,10 @@
     <t>01d8021686</t>
   </si>
   <si>
-    <t>Vietcombank</t>
-  </si>
-  <si>
     <t>NGUYỄN BÁ BA</t>
   </si>
   <si>
     <t>105881679913</t>
-  </si>
-  <si>
-    <t>TRẦN VĂN VƯƠNG</t>
-  </si>
-  <si>
-    <t>LÝ TỬ HẠ</t>
-  </si>
-  <si>
-    <t>00999</t>
-  </si>
-  <si>
-    <t>Ma kiếm</t>
-  </si>
-  <si>
-    <t>LÂM TIỂU BẠCH</t>
-  </si>
-  <si>
-    <t>000999</t>
-  </si>
-  <si>
-    <t>Thiên ma khải</t>
-  </si>
-  <si>
-    <t>PHONG VÂN MÔNG NHIÊN</t>
-  </si>
-  <si>
-    <t>000111</t>
-  </si>
-  <si>
-    <t>ĐỘC CÔ CẦU BẠI</t>
-  </si>
-  <si>
-    <t>0999999</t>
-  </si>
-  <si>
-    <t>HẢI PHAN</t>
-  </si>
-  <si>
-    <t>123321</t>
-  </si>
-  <si>
-    <t>0234</t>
-  </si>
-  <si>
-    <t>1111111</t>
-  </si>
-  <si>
-    <t>aaaaa</t>
-  </si>
-  <si>
-    <t>22222222</t>
-  </si>
-  <si>
-    <t>bbbbb</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCE07E-0643-476E-9C29-D6F951414B39}">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B77" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3542,1454 +3485,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>254</v>
+        <v>348</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>255</v>
+        <v>349</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>51</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J52" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>52</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J53" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>53</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>54</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J55" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J56" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>56</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>57</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="J58" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="K58" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>58</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J59" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K59" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>59</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J60" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N60" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J61" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N61" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="J62" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="K62" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>62</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="J63" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N63" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
-        <v>63</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J64" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N64" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>64</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J65" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L65" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M65" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N65" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>65</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J66" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K66" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M66" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N66" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>66</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J67" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L67" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M67" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N67" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>67</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="G68" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J68" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L68" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M68" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N68" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="O68" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="P68" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>68</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J69" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L69" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
-        <v>69</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J70" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M70" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="N70" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>70</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="G71" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J71" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N71" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
-        <v>71</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="G72" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J72" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L72" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="2">
-        <v>72</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J73" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L73" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
-        <v>73</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J74" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L74" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
-        <v>74</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J75" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L75" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N75" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
-        <v>75</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J76" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M76" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="N76" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <v>76</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="G77" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L77" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M77" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N77" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <v>77</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="G78" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J78" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L78" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M78" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="N78" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>78</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J79" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L79" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M79" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N79" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>79</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="G80" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J80" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M80" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>80</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J81" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L81" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M81" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N81" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
-        <v>81</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J82" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K82" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L82" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M82" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N82" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
-        <v>82</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J83" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M83" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N83" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
-        <v>83</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="G84" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J84" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="L84" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M84" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N84" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
-        <v>84</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J85" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="L85" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M85" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="N85" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -5008,8 +3515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5781,7 +4288,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
finalized app version 6.0 - minor fix form UI - minor update export function
</commit_message>
<xml_diff>
--- a/sourceDocs/THONG_TIN.xlsx
+++ b/sourceDocs/THONG_TIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\testProject\auto-complete-docx-form\sourceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F21A70F-2474-4113-8B7E-21CCD0F194D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95061334-5CB4-401D-A889-9E95E0FB7EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1466,7 +1466,7 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>